<commit_message>
test with SDES population ; EMP 2019 results
</commit_message>
<xml_diff>
--- a/test/test_insee/output/Comparaison_CSP.xlsx
+++ b/test/test_insee/output/Comparaison_CSP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.girot\.1python\mobility\test\test_insee\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC87BC59-672A-49D8-A55B-3E06F7DBA1BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24597A90-DCAA-49BA-AD77-0134359F52DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19776" windowHeight="9300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19776" windowHeight="9300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparaison 09" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>CSP : 1</t>
   </si>
@@ -47,25 +47,13 @@
     <t>CSP : 8</t>
   </si>
   <si>
-    <t>dist/trips : weekday</t>
-  </si>
-  <si>
     <t>Données EMP 2019</t>
-  </si>
-  <si>
-    <t>trips/day: weekday (jours ouvrés - jours voyage pro)</t>
   </si>
   <si>
     <t xml:space="preserve">Données EMP 2019 </t>
   </si>
   <si>
-    <t>Variation : dist/ trips weekday</t>
-  </si>
-  <si>
     <t>trips/day: weekday (jours ouvrés- voyage pro)</t>
-  </si>
-  <si>
-    <t>travel dist/y (long trips)</t>
   </si>
   <si>
     <t>Variation (jours ouvrés -jours voyage pros )</t>
@@ -105,6 +93,30 @@
   </si>
   <si>
     <t>Variation  2009 dist/ trips weekday (p_car)</t>
+  </si>
+  <si>
+    <t>trips/day: weekday (jours ouvrés - jours voyage pro) SDES pop</t>
+  </si>
+  <si>
+    <t>Variation SDES (jours ouvrés -jours voyage pros )</t>
+  </si>
+  <si>
+    <t>dist/trips : weekday INSEE</t>
+  </si>
+  <si>
+    <t>dist/trips : weekday SDES</t>
+  </si>
+  <si>
+    <t>travel dist/y (long trips) INSEE</t>
+  </si>
+  <si>
+    <t>Variation SDES : dist/ trips weekday</t>
+  </si>
+  <si>
+    <t>travel dist/y (long trips) SDES</t>
+  </si>
+  <si>
+    <t>csp</t>
   </si>
 </sst>
 </file>
@@ -662,7 +674,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -692,6 +704,8 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="43" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20 % - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1710,9 +1724,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Variation 2018 : dist/ trips weekday</a:t>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Variation</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" baseline="0"/>
+              <a:t> 2018: ntrips/weekday</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1757,12 +1776,9 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Comparaison 18'!$A$8</c:f>
+              <c:f>'Comparaison 18'!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Variation : dist/ trips weekday</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -1776,42 +1792,127 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Comparaison 18'!$B$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>CSP : 3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>CSP : 4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>CSP : 5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>CSP : 6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>CSP :7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>CSP : 8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Comparaison 18'!$B$8:$I$8</c:f>
+              <c:f>'Comparaison 18'!$B$5:$G$5</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>-3.3311183855375015E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.12986653656571567</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7.1928324959923629E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.1959383421606988E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.10027065183580675</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.5458575055608677E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6.118314328352259E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.49356080653731849</c:v>
-                </c:pt>
+                <c:ptCount val="6"/>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-80F7-4535-80A8-786BCB29C85F}"/>
+              <c16:uniqueId val="{00000000-B1B6-4F67-8179-F06F1D5BDA77}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Comparaison 18'!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Variation SDES (jours ouvrés -jours voyage pros )</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Comparaison 18'!$B$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>CSP : 3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>CSP : 4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>CSP : 5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>CSP : 6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>CSP :7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>CSP : 8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Comparaison 18'!$B$6:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.1213584058017001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.9420597017751255E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.2371010761445671E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.151223445416762E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.13371024787344998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0495020325399738E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B1B6-4F67-8179-F06F1D5BDA77}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1825,11 +1926,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="625311576"/>
-        <c:axId val="625303704"/>
+        <c:axId val="488541904"/>
+        <c:axId val="467678216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="625311576"/>
+        <c:axId val="488541904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1872,7 +1973,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="625303704"/>
+        <c:crossAx val="467678216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1880,7 +1981,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="625303704"/>
+        <c:axId val="467678216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1931,7 +2032,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="625311576"/>
+        <c:crossAx val="488541904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1943,8 +2044,46 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -2014,17 +2153,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Variation</a:t>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Variatio</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> 2018 </a:t>
+              <a:rPr lang="fr-FR" baseline="0"/>
+              <a:t>n 2018 : dist/trip weekday</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>travel dist/y (long trips)</a:t>
-            </a:r>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2059,17 +2195,7 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="9.1974783932794429E-2"/>
-          <c:y val="0.2145498783454988"/>
-          <c:w val="0.84677593479849622"/>
-          <c:h val="0.73192214111922149"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -2082,9 +2208,6 @@
               <c:f>'Comparaison 18'!$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>travel dist/y (long trips)</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -2098,42 +2221,127 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Comparaison 18'!$B$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>CSP : 3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>CSP : 4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>CSP : 5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>CSP : 6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>CSP :7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>CSP : 8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Comparaison 18'!$B$12:$I$12</c:f>
+              <c:f>'Comparaison 18'!$B$12:$G$12</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>-0.27945964611987584</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.6733921996528149E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.1379622721181546E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-9.6217071525733222E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-7.9201910465014569E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-0.2553852721474249</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-0.16108598312027311</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.3877603659034738E-2</c:v>
-                </c:pt>
+                <c:ptCount val="6"/>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D152-4A44-9E97-AB3E8A3A6E78}"/>
+              <c16:uniqueId val="{00000000-1CCC-4FAB-852A-4363D306180B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Comparaison 18'!$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Variation SDES : dist/ trips weekday</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Comparaison 18'!$B$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>CSP : 3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>CSP : 4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>CSP : 5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>CSP : 6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>CSP :7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>CSP : 8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Comparaison 18'!$B$13:$G$13</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>4.1338240789321468E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-4.1030740091495543E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-4.3933339211650102E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-6.722256698693041E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-2.1170495002901357E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2476789225340732</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1CCC-4FAB-852A-4363D306180B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2147,11 +2355,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="222711136"/>
-        <c:axId val="222697032"/>
+        <c:axId val="492262152"/>
+        <c:axId val="492262480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="222711136"/>
+        <c:axId val="492262152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2194,7 +2402,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="222697032"/>
+        <c:crossAx val="492262480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2202,7 +2410,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="222697032"/>
+        <c:axId val="492262480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2253,7 +2461,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="222711136"/>
+        <c:crossAx val="492262152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2265,8 +2473,46 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -2336,20 +2582,17 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Variation 2018 (jours ouvrés -jours voyage pros )</a:t>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Variation</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" baseline="0"/>
+              <a:t> 2018 : travel dist/year </a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.19065577411410484"/>
-          <c:y val="4.1695621959694229E-2"/>
-        </c:manualLayout>
-      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2391,12 +2634,9 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Comparaison 18'!$A$4</c:f>
+              <c:f>'Comparaison 18'!$A$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Variation (jours ouvrés -jours voyage pros )</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -2410,42 +2650,127 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Comparaison 18'!$B$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>CSP : 3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>CSP : 4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>CSP : 5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>CSP : 6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>CSP :7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>CSP : 8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Comparaison 18'!$B$4:$I$4</c:f>
+              <c:f>'Comparaison 18'!$B$18:$G$18</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0.10928093645484793</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.0623700623699843E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.11493006993006971</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.1179148737286582E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.5934065934065682E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.825791855203529E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.13913461538461247</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.0764754884201588E-2</c:v>
-                </c:pt>
+                <c:ptCount val="6"/>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2C4E-48A1-913E-8CC581BCADB5}"/>
+              <c16:uniqueId val="{00000000-9763-4F4D-ADCA-E836504629F0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Comparaison 18'!$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>travel dist/y (long trips) SDES</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Comparaison 18'!$B$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>CSP : 3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>CSP : 4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>CSP : 5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>CSP : 6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>CSP :7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>CSP : 8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Comparaison 18'!$B$19:$G$19</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>-2.096158245282298E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.1719774439955644E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-5.5003420718676699E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3405120916419886E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-6.7832294883411581E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.041803199833649E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9763-4F4D-ADCA-E836504629F0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2459,11 +2784,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="483075376"/>
-        <c:axId val="483077016"/>
+        <c:axId val="492281504"/>
+        <c:axId val="492283144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="483075376"/>
+        <c:axId val="492281504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2506,7 +2831,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="483077016"/>
+        <c:crossAx val="492283144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2514,7 +2839,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="483077016"/>
+        <c:axId val="492283144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2565,7 +2890,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="483075376"/>
+        <c:crossAx val="492281504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2577,8 +2902,46 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -6095,16 +6458,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>68581</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>232554</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>297181</xdr:rowOff>
+      <xdr:rowOff>337596</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>472440</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>636606</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>43816</xdr:rowOff>
+      <xdr:rowOff>395468</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -6119,8 +6482,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13470256" y="478156"/>
-          <a:ext cx="2775584" cy="1384935"/>
+          <a:off x="12058022" y="520862"/>
+          <a:ext cx="3567799" cy="1871239"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6155,18 +6518,8 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>rectifications apportées</a:t>
-          </a:r>
-          <a:r>
             <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
-            <a:t> : </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
-            <a:t>pondération annuelle des voyages</a:t>
+            <a:t>Hypothèses: </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -6178,19 +6531,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
-            <a:t>sample d'individus "pesés"</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
-            <a:t>calcul sur 1000 individus </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
-            <a:t>attention : résultats sans p_car ( résultats avec p _car sur 100 personnes semblait satisfaisant)                                                         </a:t>
+            <a:t>calcul sur 990 individus  sdes </a:t>
           </a:r>
           <a:endParaRPr lang="fr-FR" sz="1100"/>
         </a:p>
@@ -6200,23 +6541,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>86679</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>238125</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>558165</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>158115</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>611504</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>135255</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Graphique 3">
+        <xdr:cNvPr id="5" name="Graphique 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF6A8673-530E-4F97-9733-753760041850}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACEFD611-2073-4BB8-956B-6C80B7F27158}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6236,23 +6577,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>18098</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>29079</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>278885</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>676275</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>659315</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>89021</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Graphique 5">
+        <xdr:cNvPr id="8" name="Graphique 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0855120-051C-4898-8CA7-664C35A600A8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A520EEBB-24BE-4F4E-8265-7AB7EF085AC6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6272,23 +6613,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>200024</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>247650</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>40066</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>182637</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>634365</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>354164</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>46112</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Graphique 6">
+        <xdr:cNvPr id="9" name="Graphique 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C66B621E-467A-4465-8E56-35D73261D7DA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86B197C5-4034-4752-BEA4-086B4A9BB04E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6608,7 +6949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{655CE2B7-3B9A-45E2-A730-FF4E14DE1CB0}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
@@ -6647,7 +6988,7 @@
     </row>
     <row r="2" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1">
         <v>3.81008952515579</v>
@@ -6674,12 +7015,12 @@
         <v>2.9834745845675701</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B3" s="7">
         <v>4</v>
@@ -6710,7 +7051,7 @@
     </row>
     <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2">
         <f t="shared" ref="B4:H4" si="0">B2/B$3 -1</f>
@@ -6751,7 +7092,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1">
         <v>7.8240887471828202</v>
@@ -6781,7 +7122,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="7">
         <v>7.3</v>
@@ -6812,7 +7153,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B8" s="11">
         <f t="shared" ref="B8:I8" si="1">B6/B7-1</f>
@@ -6856,7 +7197,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B11">
         <v>1381.34</v>
@@ -6886,7 +7227,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B12" s="7">
         <v>4147</v>
@@ -6916,7 +7257,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B13" s="2">
         <f>B11/B12-1</f>
@@ -6954,15 +7295,15 @@
     <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="17" spans="2:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C17" s="8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C18" s="9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -7069,147 +7410,104 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68D27387-EB91-4065-A3EC-E947CD964524}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView topLeftCell="E3" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="D2" zoomScale="80" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="7">
-        <v>5.1026923076923003</v>
-      </c>
-      <c r="C2" s="7">
-        <v>4.0353076923076898</v>
-      </c>
-      <c r="D2" s="7">
-        <v>3.6792692307692301</v>
-      </c>
-      <c r="E2" s="7">
-        <v>3.9263628503279602</v>
-      </c>
-      <c r="F2" s="7">
-        <v>3.6607692307692301</v>
-      </c>
-      <c r="G2" s="7">
-        <v>3.4620769230769199</v>
-      </c>
-      <c r="H2" s="7">
-        <v>2.73392307692307</v>
-      </c>
-      <c r="I2" s="7">
-        <v>2.88011538461538</v>
-      </c>
-      <c r="J2" s="14" t="s">
+    <row r="2" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="B3" s="1">
+        <v>3.7004827391456101</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3.8828562089656802</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3.6482985376650601</v>
+      </c>
+      <c r="E3" s="1">
+        <v>3.50714159714417</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2.7209045948962798</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2.9078412100937299</v>
+      </c>
+      <c r="H3" s="14"/>
     </row>
-    <row r="3" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="C3">
+    <row r="4" spans="1:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>3.3</v>
+      </c>
+      <c r="C4">
         <v>3.7</v>
       </c>
-      <c r="D3">
-        <v>3.3</v>
-      </c>
-      <c r="E3">
-        <v>3.7</v>
-      </c>
-      <c r="F3">
+      <c r="D4">
         <v>3.5</v>
       </c>
-      <c r="G3">
+      <c r="E4">
         <v>3.4</v>
       </c>
-      <c r="H3">
+      <c r="F4">
         <v>2.4</v>
       </c>
-      <c r="I3" s="6">
+      <c r="G4" s="6">
         <f>(3209*3.2+ 11936*2.8 + 2144*2.6)/(3209+11936+2144)</f>
         <v>2.8494418416334084</v>
       </c>
-      <c r="J3" s="14"/>
+      <c r="H4" s="14"/>
     </row>
-    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="2">
-        <f t="shared" ref="B4:I4" si="0">B2/B$3 -1</f>
-        <v>0.10928093645484793</v>
-      </c>
-      <c r="C4" s="2">
-        <f t="shared" si="0"/>
-        <v>9.0623700623699843E-2</v>
-      </c>
-      <c r="D4" s="2">
-        <f t="shared" si="0"/>
-        <v>0.11493006993006971</v>
-      </c>
-      <c r="E4" s="2">
-        <f t="shared" si="0"/>
-        <v>6.1179148737286582E-2</v>
-      </c>
-      <c r="F4" s="2">
-        <f t="shared" si="0"/>
-        <v>4.5934065934065682E-2</v>
-      </c>
-      <c r="G4" s="2">
-        <f t="shared" si="0"/>
-        <v>1.825791855203529E-2</v>
-      </c>
-      <c r="H4" s="2">
-        <f t="shared" si="0"/>
-        <v>0.13913461538461247</v>
-      </c>
-      <c r="I4" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0764754884201588E-2</v>
-      </c>
-      <c r="J4" s="14"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -7217,221 +7515,301 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="14"/>
+      <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="2">
+        <f t="shared" ref="B6:G6" si="0">B3/B$4 -1</f>
+        <v>0.1213584058017001</v>
+      </c>
+      <c r="C6" s="2">
+        <f t="shared" si="0"/>
+        <v>4.9420597017751255E-2</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="0"/>
+        <v>4.2371010761445671E-2</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>3.151223445416762E-2</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.13371024787344998</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>2.0495020325399738E-2</v>
+      </c>
+      <c r="H6" s="14"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="14"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="14"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="7">
+        <v>12.6487542345271</v>
+      </c>
+      <c r="C9" s="7">
+        <v>12.1909247860328</v>
+      </c>
+      <c r="D9" s="7">
+        <v>9.9024358665222607</v>
+      </c>
+      <c r="E9" s="7">
+        <v>11.907773613139501</v>
+      </c>
+      <c r="F9" s="7">
+        <v>7.5344003173130103</v>
+      </c>
+      <c r="G9" s="7">
+        <v>9.3246001404702206</v>
+      </c>
+      <c r="H9" s="14"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1">
+        <v>11.848779124131401</v>
+      </c>
+      <c r="C10" s="1">
+        <v>11.219940340929501</v>
+      </c>
+      <c r="D10" s="1">
+        <v>8.6045999470951493</v>
+      </c>
+      <c r="E10" s="1">
+        <v>10.726940479650301</v>
+      </c>
+      <c r="F10" s="1">
+        <v>6.9496894854794</v>
+      </c>
+      <c r="G10" s="1">
+        <v>7.7895101460887597</v>
+      </c>
+      <c r="H10" s="14"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="7">
-        <v>6.1868084233256004</v>
-      </c>
-      <c r="C6" s="7">
-        <v>12.3155452485663</v>
-      </c>
-      <c r="D6" s="7">
-        <v>12.6487542345271</v>
-      </c>
-      <c r="E6" s="7">
-        <v>12.1909247860328</v>
-      </c>
-      <c r="F6" s="7">
-        <v>9.9024358665222607</v>
-      </c>
-      <c r="G6" s="7">
-        <v>11.907773613139501</v>
-      </c>
-      <c r="H6" s="7">
-        <v>7.5344003173130103</v>
-      </c>
-      <c r="I6" s="7">
-        <v>9.3246001404702206</v>
-      </c>
-      <c r="J6" s="14"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B11">
+        <v>11.8</v>
+      </c>
+      <c r="C11">
+        <v>11.7</v>
+      </c>
+      <c r="D11">
         <v>9</v>
       </c>
-      <c r="B7">
-        <v>6.4</v>
-      </c>
-      <c r="C7">
-        <v>10.9</v>
-      </c>
-      <c r="D7">
-        <v>11.8</v>
-      </c>
-      <c r="E7">
-        <v>11.7</v>
-      </c>
-      <c r="F7">
-        <v>9</v>
-      </c>
-      <c r="G7">
+      <c r="E11">
         <v>11.5</v>
       </c>
-      <c r="H7">
+      <c r="F11">
         <v>7.1</v>
       </c>
-      <c r="I7" s="1">
+      <c r="G11" s="1">
         <f>(3209*6.7+ 11936*6.2 + 2144*5.8)/(3209+11936+2144)</f>
         <v>6.2432008791717273</v>
       </c>
-      <c r="J7" s="14"/>
+      <c r="H11" s="14"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="3">
-        <f>B6/B7-1</f>
-        <v>-3.3311183855375015E-2</v>
-      </c>
-      <c r="C8" s="3">
-        <f t="shared" ref="C8:I8" si="1">C6/C7-1</f>
-        <v>0.12986653656571567</v>
-      </c>
-      <c r="D8" s="3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="14"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="3">
+        <f t="shared" ref="B13:G13" si="1">B10/B11-1</f>
+        <v>4.1338240789321468E-3</v>
+      </c>
+      <c r="C13" s="3">
         <f t="shared" si="1"/>
-        <v>7.1928324959923629E-2</v>
-      </c>
-      <c r="E8" s="3">
+        <v>-4.1030740091495543E-2</v>
+      </c>
+      <c r="D13" s="3">
         <f t="shared" si="1"/>
-        <v>4.1959383421606988E-2</v>
-      </c>
-      <c r="F8" s="3">
+        <v>-4.3933339211650102E-2</v>
+      </c>
+      <c r="E13" s="3">
         <f t="shared" si="1"/>
-        <v>0.10027065183580675</v>
-      </c>
-      <c r="G8" s="3">
+        <v>-6.722256698693041E-2</v>
+      </c>
+      <c r="F13" s="3">
         <f t="shared" si="1"/>
-        <v>3.5458575055608677E-2</v>
-      </c>
-      <c r="H8" s="3">
+        <v>-2.1170495002901357E-2</v>
+      </c>
+      <c r="G13" s="3">
         <f t="shared" si="1"/>
-        <v>6.118314328352259E-2</v>
-      </c>
-      <c r="I8" s="3">
-        <f t="shared" si="1"/>
-        <v>0.49356080653731849</v>
-      </c>
-      <c r="J8" s="14"/>
+        <v>0.2476789225340732</v>
+      </c>
+      <c r="H13" s="12"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J9" s="12"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="15"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="12"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="7">
-        <v>2784.1679273927998</v>
-      </c>
-      <c r="C10" s="7">
-        <v>15255.1001791774</v>
-      </c>
-      <c r="D10" s="7">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="7">
         <v>19519.5859698245</v>
       </c>
-      <c r="E10" s="7">
+      <c r="C15" s="7">
         <v>9362.2873560649296</v>
       </c>
-      <c r="F10" s="7">
+      <c r="D15" s="7">
         <v>5685.0074047890002</v>
       </c>
-      <c r="G10" s="7">
+      <c r="E15" s="7">
         <v>3319.4924567667799</v>
       </c>
-      <c r="H10" s="7">
+      <c r="F15" s="7">
         <v>4330.4741551331499</v>
       </c>
-      <c r="I10" s="7">
+      <c r="G15" s="7">
         <v>6869.8039510797098</v>
       </c>
-      <c r="J10" s="14" t="s">
-        <v>25</v>
+      <c r="H15" s="14" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="5">
-        <v>3864</v>
-      </c>
-      <c r="C11" s="5">
-        <v>14574</v>
-      </c>
-      <c r="D11" s="5">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="5">
+        <v>18710.403197744101</v>
+      </c>
+      <c r="C16" s="5">
+        <v>10237.594856576499</v>
+      </c>
+      <c r="D16" s="5">
+        <v>5834.4088804828898</v>
+      </c>
+      <c r="E16" s="5">
+        <v>4562.3400290454001</v>
+      </c>
+      <c r="F16" s="5">
+        <v>4811.8496938118296</v>
+      </c>
+      <c r="G16" s="5">
+        <v>6594.3496598396296</v>
+      </c>
+      <c r="H16" s="14"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="5">
         <v>19111</v>
       </c>
-      <c r="E11" s="5">
+      <c r="C17" s="5">
         <v>10359</v>
       </c>
-      <c r="F11" s="5">
+      <c r="D17" s="5">
         <v>6174</v>
       </c>
-      <c r="G11" s="5">
+      <c r="E17" s="5">
         <v>4458</v>
       </c>
-      <c r="H11" s="5">
+      <c r="F17" s="5">
         <v>5162</v>
       </c>
-      <c r="I11" s="5">
+      <c r="G17" s="5">
         <f>(3209*6596+ 11936*6550 + 2144*4773)/(3209+11936+2144)</f>
         <v>6338.1731736942565</v>
       </c>
-      <c r="J11" s="14"/>
+      <c r="H17" s="14"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="2">
-        <f t="shared" ref="B12:I12" si="2">B10/B11-1</f>
-        <v>-0.27945964611987584</v>
-      </c>
-      <c r="C12" s="2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="14"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="2">
+        <f>B16/B17-1</f>
+        <v>-2.096158245282298E-2</v>
+      </c>
+      <c r="C19" s="2">
+        <f t="shared" ref="C19:G19" si="2">C16/C17-1</f>
+        <v>-1.1719774439955644E-2</v>
+      </c>
+      <c r="D19" s="2">
         <f t="shared" si="2"/>
-        <v>4.6733921996528149E-2</v>
-      </c>
-      <c r="D12" s="2">
+        <v>-5.5003420718676699E-2</v>
+      </c>
+      <c r="E19" s="2">
         <f t="shared" si="2"/>
-        <v>2.1379622721181546E-2</v>
-      </c>
-      <c r="E12" s="2">
+        <v>2.3405120916419886E-2</v>
+      </c>
+      <c r="F19" s="2">
         <f t="shared" si="2"/>
-        <v>-9.6217071525733222E-2</v>
-      </c>
-      <c r="F12" s="2">
+        <v>-6.7832294883411581E-2</v>
+      </c>
+      <c r="G19" s="2">
         <f t="shared" si="2"/>
-        <v>-7.9201910465014569E-2</v>
-      </c>
-      <c r="G12" s="2">
-        <f t="shared" si="2"/>
-        <v>-0.2553852721474249</v>
-      </c>
-      <c r="H12" s="2">
-        <f t="shared" si="2"/>
-        <v>-0.16108598312027311</v>
-      </c>
-      <c r="I12" s="2">
-        <f t="shared" si="2"/>
-        <v>8.3877603659034738E-2</v>
-      </c>
-      <c r="J12" s="14"/>
+        <v>4.041803199833649E-2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="J2:J8"/>
-    <mergeCell ref="J10:J12"/>
+    <mergeCell ref="H2:H12"/>
+    <mergeCell ref="H15:H18"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="J2:J8" r:id="rId1" display="référence: feuille 7" xr:uid="{0127559A-7101-4CE1-805C-928394CB1E2A}"/>
-    <hyperlink ref="J10:J12" r:id="rId2" display="référence: feuille 1" xr:uid="{6DCF3343-2233-4304-B8CB-20F9A073FD33}"/>
+    <hyperlink ref="H2:H12" r:id="rId1" display="référence: feuille 7" xr:uid="{0127559A-7101-4CE1-805C-928394CB1E2A}"/>
+    <hyperlink ref="H15:H18" r:id="rId2" display="référence: feuille 1" xr:uid="{6DCF3343-2233-4304-B8CB-20F9A073FD33}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId3"/>

</xml_diff>

<commit_message>
Compare computed with results with EMP results : SDES population
</commit_message>
<xml_diff>
--- a/test/test_insee/output/Comparaison_CSP.xlsx
+++ b/test/test_insee/output/Comparaison_CSP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.girot\.1python\mobility\test\test_insee\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24597A90-DCAA-49BA-AD77-0134359F52DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D43BAA-9DDD-4418-BE33-D95169E48FA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19776" windowHeight="9300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -701,11 +701,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="43" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20 % - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -7014,7 +7014,7 @@
       <c r="I2" s="1">
         <v>2.9834745845675701</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="16" t="s">
         <v>15</v>
       </c>
     </row>
@@ -7047,7 +7047,7 @@
         <f>(2338*3.1+ 11808*3 + 3407*2.8)/(2338+11808+3407)</f>
         <v>2.9745000854554777</v>
       </c>
-      <c r="J3" s="14"/>
+      <c r="J3" s="16"/>
     </row>
     <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -7085,10 +7085,10 @@
         <f>I2/I$3-1</f>
         <v>3.017145353592543E-3</v>
       </c>
-      <c r="J4" s="14"/>
+      <c r="J4" s="16"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J5" s="14"/>
+      <c r="J5" s="16"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -7118,7 +7118,7 @@
       <c r="I6" s="1">
         <v>8.2138636453465192</v>
       </c>
-      <c r="J6" s="14"/>
+      <c r="J6" s="16"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -7149,7 +7149,7 @@
         <f>(2338*6.5+ 11808*6 + 3407*5.6)/(2338+11808+3407)</f>
         <v>5.9889591522816614</v>
       </c>
-      <c r="J7" s="14"/>
+      <c r="J7" s="16"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -7223,7 +7223,7 @@
       <c r="I11">
         <v>3309.68</v>
       </c>
-      <c r="J11" s="14"/>
+      <c r="J11" s="16"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -7253,7 +7253,7 @@
       <c r="I12" s="7">
         <v>4247</v>
       </c>
-      <c r="J12" s="14"/>
+      <c r="J12" s="16"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -7412,7 +7412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68D27387-EB91-4065-A3EC-E947CD964524}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" zoomScale="80" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E2" zoomScale="80" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
@@ -7454,7 +7454,7 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="16" t="s">
         <v>20</v>
       </c>
     </row>
@@ -7480,7 +7480,7 @@
       <c r="G3" s="1">
         <v>2.9078412100937299</v>
       </c>
-      <c r="H3" s="14"/>
+      <c r="H3" s="16"/>
     </row>
     <row r="4" spans="1:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -7505,7 +7505,7 @@
         <f>(3209*3.2+ 11936*2.8 + 2144*2.6)/(3209+11936+2144)</f>
         <v>2.8494418416334084</v>
       </c>
-      <c r="H4" s="14"/>
+      <c r="H4" s="16"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
@@ -7515,7 +7515,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="14"/>
+      <c r="H5" s="16"/>
     </row>
     <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
@@ -7545,7 +7545,7 @@
         <f t="shared" si="0"/>
         <v>2.0495020325399738E-2</v>
       </c>
-      <c r="H6" s="14"/>
+      <c r="H6" s="16"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
@@ -7555,7 +7555,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="14"/>
+      <c r="H7" s="16"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
@@ -7565,7 +7565,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="14"/>
+      <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -7589,7 +7589,7 @@
       <c r="G9" s="7">
         <v>9.3246001404702206</v>
       </c>
-      <c r="H9" s="14"/>
+      <c r="H9" s="16"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -7613,7 +7613,7 @@
       <c r="G10" s="1">
         <v>7.7895101460887597</v>
       </c>
-      <c r="H10" s="14"/>
+      <c r="H10" s="16"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -7638,7 +7638,7 @@
         <f>(3209*6.7+ 11936*6.2 + 2144*5.8)/(3209+11936+2144)</f>
         <v>6.2432008791717273</v>
       </c>
-      <c r="H11" s="14"/>
+      <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
@@ -7647,7 +7647,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="14"/>
+      <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -7680,13 +7680,13 @@
       <c r="H13" s="12"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
       <c r="H14" s="12"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -7711,7 +7711,7 @@
       <c r="G15" s="7">
         <v>6869.8039510797098</v>
       </c>
-      <c r="H15" s="14" t="s">
+      <c r="H15" s="16" t="s">
         <v>21</v>
       </c>
     </row>
@@ -7737,7 +7737,7 @@
       <c r="G16" s="5">
         <v>6594.3496598396296</v>
       </c>
-      <c r="H16" s="14"/>
+      <c r="H16" s="16"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -7762,7 +7762,7 @@
         <f>(3209*6596+ 11936*6550 + 2144*4773)/(3209+11936+2144)</f>
         <v>6338.1731736942565</v>
       </c>
-      <c r="H17" s="14"/>
+      <c r="H17" s="16"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
@@ -7771,7 +7771,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="14"/>
+      <c r="H18" s="16"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">

</xml_diff>